<commit_message>
Revert "Improved the Excel output to have multiple sheets"
This reverts commit cc1d77271d48b996555e4ef7751b7e5c9fdbdb59.
</commit_message>
<xml_diff>
--- a/InnovoWebApps Facebook Data.xlsx
+++ b/InnovoWebApps Facebook Data.xlsx
@@ -7,10 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Posts" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Words" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Hashtags" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Comments" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -419,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:N98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +435,9 @@
     <col width="8.26" customWidth="1" min="9" max="9"/>
     <col width="8.26" customWidth="1" min="10" max="10"/>
     <col width="20.63" customWidth="1" min="11" max="11"/>
+    <col width="8.26" customWidth="1" min="12" max="12"/>
+    <col width="8.26" customWidth="1" min="13" max="13"/>
+    <col width="15.53" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -496,6 +496,21 @@
           <t>Caption</t>
         </is>
       </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Words</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Hashtags</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Comments Text</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -544,16 +559,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/150229681095877/posts/150095501109295</t>
+          <t>https://www.facebook.com/150229681095877/posts/150095221109323?substory_index=1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://scontent-lax3-2.xx.fbcdn.net/v/t39.30808-6/320235597_5842691565785954_7399001920670591574_n.png?stp=dst-png_s720x720&amp;_nc_cat=111&amp;ccb=1-7&amp;_nc_sid=dd9801&amp;_nc_ohc=aXyU2Fz8ilsAX-YAUhF&amp;_nc_ht=scontent-lax3-2.xx&amp;edm=AO-AMGsEAAAA&amp;oh=00_AfCrAtHACxhQzAgTrYrJ3kxPirbBdMzGPBEFjPDS3SkAUQ&amp;oe=63A16890</t>
+          <t>https://scontent-lax3-2.xx.fbcdn.net/v/t39.30808-6/320226857_1311606946306014_1482705118669418596_n.jpg?stp=dst-jpg_p720x720&amp;_nc_cat=107&amp;ccb=1-7&amp;_nc_sid=85a577&amp;_nc_ohc=xoMNmBITxykAX9o_Y6A&amp;_nc_ht=scontent-lax3-2.xx&amp;edm=AO-AMGsEAAAA&amp;oh=00_AfCsOSb0FSKBFD-m802f9yU_ujuQP8gBENUUurpGa4S5_g&amp;oe=639F8DE1</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
@@ -566,7 +581,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>3:14:10</t>
+          <t>3:22:08</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -581,7 +596,7 @@
       <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>null</t>
         </is>
@@ -589,16 +604,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/150229681095877/posts/150095221109323?substory_index=0</t>
+          <t>https://www.facebook.com/150229681095877/posts/150095501109295</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://scontent-lax3-2.xx.fbcdn.net/v/t39.30808-6/320225569_1292682331518752_6149852901690901064_n.jpg?_nc_cat=100&amp;ccb=1-7&amp;_nc_sid=7aed08&amp;_nc_ohc=UtRpmFSp2DYAX8doLvP&amp;_nc_oc=AQkd95LSXCaNuAobUQvsRpEKEMlAxMy-kGxrfN8eCAfiYIh07joBw82orAQiol3j93M&amp;_nc_ht=scontent-lax3-2.xx&amp;edm=AO-AMGsEAAAA&amp;oh=00_AfAYEcMUi4ScRtubI-TrYMccXn5W_fQeA6i5O3DDC4HEJw&amp;oe=63A0B5B0</t>
+          <t>https://scontent-lax3-2.xx.fbcdn.net/v/t39.30808-6/320235597_5842691565785954_7399001920670591574_n.png?stp=dst-png_s720x720&amp;_nc_cat=111&amp;ccb=1-7&amp;_nc_sid=dd9801&amp;_nc_ohc=aXyU2Fz8ilsAX-YAUhF&amp;_nc_ht=scontent-lax3-2.xx&amp;edm=AO-AMGsEAAAA&amp;oh=00_AfCrAtHACxhQzAgTrYrJ3kxPirbBdMzGPBEFjPDS3SkAUQ&amp;oe=63A16890</t>
         </is>
       </c>
       <c r="D4" s="1" t="n">
@@ -611,14 +626,14 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>3:11:43</t>
+          <t>3:14:10</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -634,126 +649,126 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137532132277310/</t>
+          <t>https://www.facebook.com/150229681095877/posts/150095501109295</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>https://scontent-lax3-2.xx.fbcdn.net/v/t39.30808-6/320235597_5842691565785954_7399001920670591574_n.png?stp=dst-png_s720x720&amp;_nc_cat=111&amp;ccb=1-7&amp;_nc_sid=dd9801&amp;_nc_ohc=aXyU2Fz8ilsAX-YAUhF&amp;_nc_ht=scontent-lax3-2.xx&amp;edm=AO-AMGsEAAAA&amp;oh=00_AfCrAtHACxhQzAgTrYrJ3kxPirbBdMzGPBEFjPDS3SkAUQ&amp;oe=63A16890</t>
         </is>
       </c>
       <c r="D5" s="1" t="n">
-        <v>44740</v>
+        <v>44910</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>4:09:43</t>
+          <t>3:14:10</t>
         </is>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Test post 101!</t>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>null</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137532122277311/</t>
+          <t>https://www.facebook.com/150229681095877/posts/150095221109323?substory_index=0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>https://scontent-lax3-2.xx.fbcdn.net/v/t39.30808-6/320225569_1292682331518752_6149852901690901064_n.jpg?_nc_cat=100&amp;ccb=1-7&amp;_nc_sid=7aed08&amp;_nc_ohc=UtRpmFSp2DYAX8doLvP&amp;_nc_oc=AQkd95LSXCaNuAobUQvsRpEKEMlAxMy-kGxrfN8eCAfiYIh07joBw82orAQiol3j93M&amp;_nc_ht=scontent-lax3-2.xx&amp;edm=AO-AMGsEAAAA&amp;oh=00_AfAYEcMUi4ScRtubI-TrYMccXn5W_fQeA6i5O3DDC4HEJw&amp;oe=63A0B5B0</t>
         </is>
       </c>
       <c r="D6" s="1" t="n">
-        <v>44740</v>
+        <v>44910</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>4:09:35</t>
+          <t>3:11:43</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Test post 100!!</t>
+          <t>null</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137532088943981/</t>
+          <t>https://www.facebook.com/150229681095877/posts/150095221109323?substory_index=0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>https://scontent-lax3-2.xx.fbcdn.net/v/t39.30808-6/320225569_1292682331518752_6149852901690901064_n.jpg?_nc_cat=100&amp;ccb=1-7&amp;_nc_sid=7aed08&amp;_nc_ohc=UtRpmFSp2DYAX8doLvP&amp;_nc_oc=AQkd95LSXCaNuAobUQvsRpEKEMlAxMy-kGxrfN8eCAfiYIh07joBw82orAQiol3j93M&amp;_nc_ht=scontent-lax3-2.xx&amp;edm=AO-AMGsEAAAA&amp;oh=00_AfAYEcMUi4ScRtubI-TrYMccXn5W_fQeA6i5O3DDC4HEJw&amp;oe=63A0B5B0</t>
         </is>
       </c>
       <c r="D7" s="1" t="n">
-        <v>44740</v>
+        <v>44910</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4:09:24</t>
+          <t>3:11:43</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -761,19 +776,19 @@
       <c r="J7" t="n">
         <v>0</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Test post 99!</t>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>null</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137532075610649/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532132277310/</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -791,34 +806,34 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>4:09:17</t>
+          <t>4:09:43</t>
         </is>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Test post 98!</t>
+          <t>Test post 101!</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137532062277317/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532132277310/</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -836,34 +851,34 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>4:09:10</t>
+          <t>4:09:43</t>
         </is>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Test post 97!</t>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137532048943985/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532132277310/</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -881,34 +896,34 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>4:09:03</t>
+          <t>4:09:43</t>
         </is>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Test post 96!</t>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137532018943988/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532132277310/</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -926,34 +941,34 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>4:08:56</t>
+          <t>4:09:43</t>
         </is>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Test post 95!</t>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>101</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531978943992/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532132277310/</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -971,34 +986,34 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>4:08:49</t>
+          <t>4:09:43</t>
         </is>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Test post 94!</t>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Comment 2 on 101!</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531935610663/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532132277310/</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1016,34 +1031,34 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>4:08:35</t>
+          <t>4:09:43</t>
         </is>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Test post 93!</t>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Comment 1 on 101!</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531905610666/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532122277311/</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1061,34 +1076,34 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>4:08:28</t>
+          <t>4:09:35</t>
         </is>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Test post 92!</t>
+          <t>Test post 100!!</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531838944006/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532122277311/</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1106,34 +1121,34 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>4:08:13</t>
+          <t>4:09:35</t>
         </is>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Test post 91!</t>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531772277346/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532122277311/</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1151,34 +1166,34 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>4:08:02</t>
+          <t>4:09:35</t>
         </is>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Test post 90!</t>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531758944014/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532122277311/</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1196,34 +1211,34 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>4:07:54</t>
+          <t>4:09:35</t>
         </is>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Test post 89!</t>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531705610686/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532122277311/</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1241,34 +1256,34 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>4:07:48</t>
+          <t>4:09:35</t>
         </is>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>Test post 88!</t>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Test Comment on 100!</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531662277357/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532088943981/</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1286,7 +1301,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4:07:41</t>
+          <t>4:09:24</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1303,17 +1318,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Test post 87!</t>
+          <t>Test post 99!</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531568944033/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532088943981/</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1331,7 +1346,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>4:07:25</t>
+          <t>4:09:24</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1346,19 +1361,19 @@
       <c r="J20" t="n">
         <v>0</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>Test post 86!</t>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531528944037/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532088943981/</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1376,7 +1391,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>4:07:18</t>
+          <t>4:09:24</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1391,19 +1406,19 @@
       <c r="J21" t="n">
         <v>0</v>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Test post 85!</t>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531478944042/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532088943981/</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1421,7 +1436,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>4:07:09</t>
+          <t>4:09:24</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1436,19 +1451,19 @@
       <c r="J22" t="n">
         <v>0</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Test post 84!</t>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>99</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531422277381/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532075610649/</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1466,7 +1481,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>4:06:59</t>
+          <t>4:09:17</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1483,17 +1498,17 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Test post 83!</t>
+          <t>Test post 98!</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531372277386/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532075610649/</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1511,7 +1526,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>4:06:52</t>
+          <t>4:09:17</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1526,19 +1541,19 @@
       <c r="J24" t="n">
         <v>0</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>Test post 82!</t>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531342277389/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532075610649/</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1556,7 +1571,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>4:06:45</t>
+          <t>4:09:17</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1571,19 +1586,19 @@
       <c r="J25" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>Test post 81!</t>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/101235249240332/posts/137531295610727/</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532075610649/</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1601,7 +1616,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>4:06:38</t>
+          <t>4:09:17</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1616,352 +1631,277 @@
       <c r="J26" t="n">
         <v>0</v>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>Test post 80!</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B70"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col width="7.8" customWidth="1" min="1" max="1"/>
-    <col width="21.22" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Post_Id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Words</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>post</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>post</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>5</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>6</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>6</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>post</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>6</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>7</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>7</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>post</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>7</v>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>98</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>8</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>8</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>post</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>8</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>9</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>9</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>post</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>9</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>10</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>10</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>post</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>10</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>95</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>11</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>test</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532062277317/</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>4:09:10</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Test post 97!</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532062277317/</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>4:09:10</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532062277317/</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>4:09:10</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532062277317/</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>4:09:10</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>97</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532048943985/</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>4:09:03</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Test post 96!</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B32" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137532048943985/</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>4:09:03</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="inlineStr">
         <is>
           <t>test</t>
         </is>
@@ -1969,9 +1909,44 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137532048943985/</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>4:09:03</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="inlineStr">
         <is>
           <t>post</t>
         </is>
@@ -1979,109 +1954,494 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532048943985/</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>4:09:03</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>96</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532018943988/</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>4:08:56</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Test post 95!</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532018943988/</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>4:08:56</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532018943988/</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>4:08:56</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137532018943988/</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>4:08:56</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>95</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531978943992/</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>4:08:49</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Test post 94!</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531978943992/</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>4:08:49</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531978943992/</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>4:08:49</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531978943992/</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>4:08:49</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>94</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531935610663/</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>4:08:35</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Test post 93!</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B44" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531935610663/</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>4:08:35</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="inlineStr">
         <is>
           <t>test</t>
         </is>
@@ -2089,9 +2449,44 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B45" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531935610663/</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>4:08:35</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="inlineStr">
         <is>
           <t>post</t>
         </is>
@@ -2099,109 +2494,494 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531935610663/</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>4:08:35</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>93</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531905610666/</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>4:08:28</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Test post 92!</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531905610666/</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>4:08:28</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531905610666/</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>4:08:28</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531905610666/</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>4:08:28</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>92</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531838944006/</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>4:08:13</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Test post 91!</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531838944006/</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>4:08:13</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531838944006/</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>4:08:13</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531838944006/</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>4:08:13</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>91</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531772277346/</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>4:08:02</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Test post 90!</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B56" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531772277346/</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D56" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>4:08:02</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" t="inlineStr">
         <is>
           <t>test</t>
         </is>
@@ -2209,9 +2989,44 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B57" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531772277346/</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>4:08:02</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" t="inlineStr">
         <is>
           <t>post</t>
         </is>
@@ -2219,109 +3034,494 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531772277346/</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D58" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>4:08:02</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>90</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531758944014/</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>4:07:54</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Test post 89!</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531758944014/</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D60" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>4:07:54</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531758944014/</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>4:07:54</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531758944014/</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D62" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>4:07:54</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>89</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531705610686/</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>4:07:48</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Test post 88!</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531705610686/</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D64" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>4:07:48</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531705610686/</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>4:07:48</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>post</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531705610686/</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D66" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>4:07:48</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>88</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>https://www.facebook.com/101235249240332/posts/137531662277357/</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D67" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>4:07:41</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Test post 87!</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B68" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531662277357/</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D68" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>4:07:41</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" t="inlineStr">
         <is>
           <t>test</t>
         </is>
@@ -2329,9 +3529,44 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B69" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531662277357/</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D69" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>4:07:41</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
+      <c r="L69" t="inlineStr">
         <is>
           <t>post</t>
         </is>
@@ -2339,111 +3574,1306 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
+        <v>18</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531662277357/</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D70" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>4:07:41</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0</v>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>19</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531568944033/</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D71" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>4:07:25</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Test post 86!</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>19</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531568944033/</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D72" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>4:07:25</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>19</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531568944033/</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D73" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>4:07:25</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0</v>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>19</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531568944033/</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D74" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>4:07:25</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>20</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531528944037/</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D75" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>4:07:18</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Test post 85!</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>20</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531528944037/</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D76" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>4:07:18</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>20</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531528944037/</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D77" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>4:07:18</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>20</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531528944037/</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D78" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>4:07:18</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0</v>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>21</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531478944042/</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D79" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>4:07:09</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Test post 84!</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>21</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531478944042/</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D80" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>4:07:09</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>21</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531478944042/</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D81" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>4:07:09</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0</v>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>21</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531478944042/</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D82" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>4:07:09</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0</v>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>22</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531422277381/</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D83" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>4:06:59</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Test post 83!</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>22</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531422277381/</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D84" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>4:06:59</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0</v>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>22</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531422277381/</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D85" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>4:06:59</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>22</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531422277381/</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D86" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>4:06:59</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>23</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531372277386/</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D87" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>4:06:52</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Test post 82!</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>23</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531372277386/</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D88" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>4:06:52</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0</v>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>23</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531372277386/</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D89" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>4:06:52</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0</v>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>23</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531372277386/</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D90" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>4:06:52</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>24</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531342277389/</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D91" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>4:06:45</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Test post 81!</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>24</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531342277389/</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D92" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>4:06:45</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0</v>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>24</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531342277389/</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D93" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>4:06:45</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0</v>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>24</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531342277389/</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D94" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>4:06:45</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0</v>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
         <v>25</v>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531295610727/</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D95" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>4:06:38</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Test post 80!</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>25</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531295610727/</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D96" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>4:06:38</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>0</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0</v>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>25</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531295610727/</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D97" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>4:06:38</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0</v>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>25</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/101235249240332/posts/137531295610727/</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="D98" s="1" t="n">
+        <v>44740</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>4:06:38</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0</v>
+      </c>
+      <c r="L98" t="inlineStr">
         <is>
           <t>80</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col width="7.8" customWidth="1" min="1" max="1"/>
-    <col width="21.22" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Post_Id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Hashtags</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="7.8" customWidth="1" min="1" max="1"/>
-    <col width="21.22" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Post_Id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Words</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Comment 2 on 101!</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Comment 1 on 101!</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Test Comment on 100!</t>
         </is>
       </c>
     </row>

</xml_diff>